<commit_message>
Update tracker data 2025-07-22 17:44:31
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,32 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Maskehsjjabbajaja</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:45:12
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,32 +521,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Maskehsjjabbajaja</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:45:17
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,32 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hajjana</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:45:54
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,32 +521,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hajjana</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:46:25
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,32 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="F2" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-07-22 17:59:20
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,32 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test1jq</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45860</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:21:06
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,32 +495,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>sedrftgyhuioygtfrd</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6390549155990778</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45860</v>
-      </c>
-      <c r="F3" t="n">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update tracker data 2025-09-07 16:23:16
</commit_message>
<xml_diff>
--- a/tracker_data.xlsx
+++ b/tracker_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,12 +472,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Test1</t>
+          <t>Workout</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,24 +486,24 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6390549155990778</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45860</v>
+        <v>45907</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>G2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Workout</t>
+          <t>Eat Healthy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -524,12 +524,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>G3</t>
+          <t>G4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Eat Healthy</t>
+          <t>Read Book</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -550,12 +550,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>G4</t>
+          <t>G5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Read Book</t>
+          <t>Investment Plan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -576,17 +576,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G5</t>
+          <t>G6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Investment Plan</t>
+          <t>Spend 10 Hours without phone</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Weekly</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -596,32 +596,6 @@
         <v>45907</v>
       </c>
       <c r="F6" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>G6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Spend 10 Hours without phone</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Weekly</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>45907</v>
-      </c>
-      <c r="F7" t="n">
         <v>36</v>
       </c>
     </row>

</xml_diff>